<commit_message>
Update Selected data dictionary.xlsx
</commit_message>
<xml_diff>
--- a/Selected data dictionary.xlsx
+++ b/Selected data dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52322\OneDrive - The University of Chicago\Documents\Harris\2022 Winter\Policy Lab\Data\Colombia-Police-Reform\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uchicagoedu-my.sharepoint.com/personal/etruqui_uchicago_edu/Documents/Documents/Harris/2022 Winter/Policy Lab/Data/Colombia-Police-Reform/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19AA06E8-BC38-4EF7-9F59-F18504189BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{FAD8D356-124B-4807-A224-08D957735C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B0A7E236-6728-4073-A86A-1391BAD17152}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>COD_DANE_A</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Variable</t>
+  </si>
+  <si>
+    <t>TP19_EE_E9</t>
   </si>
 </sst>
 </file>
@@ -544,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9753C83D-E08C-4950-9775-97579C9EBA3E}">
-  <dimension ref="A1:A46"/>
+  <dimension ref="A1:A47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -644,141 +647,146 @@
     </row>
     <row r="19" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -788,6 +796,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2D1F71C56D1734C8B12A33883B3E361" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6db6bf29bcf640f53350f363ca07d85b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c27dc19d-9a14-4383-882b-19237e89b46f" xmlns:ns4="30df9d36-c0b0-4b66-af03-965086fa9095" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e84e3890b35d3d988bc9b47ac3ba3752" ns3:_="" ns4:_="">
     <xsd:import namespace="c27dc19d-9a14-4383-882b-19237e89b46f"/>
@@ -1016,22 +1039,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCE9FDB9-430A-4F32-82C4-B79AA4963E8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c27dc19d-9a14-4383-882b-19237e89b46f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="30df9d36-c0b0-4b66-af03-965086fa9095"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59A73D06-5CA0-4250-8CE0-EF1DDFCD3CE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AEAE002-2F2E-4DF7-B97E-0E9B3F68A489}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1048,29 +1081,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59A73D06-5CA0-4250-8CE0-EF1DDFCD3CE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCE9FDB9-430A-4F32-82C4-B79AA4963E8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c27dc19d-9a14-4383-882b-19237e89b46f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="30df9d36-c0b0-4b66-af03-965086fa9095"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>